<commit_message>
Add Jimmy668 for evidence
</commit_message>
<xml_diff>
--- a/2019jack/evidence.xlsx
+++ b/2019jack/evidence.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cosmos\gon-evidence\2019jack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Demo\gon-evidence\2019jack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1352DE-BA00-47BC-8B77-F9C07AF14FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
   <si>
     <t>TeamName</t>
   </si>
@@ -152,11 +151,38 @@
     <t>omniflix1jmk0t74c728v2npnpnxqkvufyyq7pw5lthn6dt</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>Jimmy668</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>iaa1tqz6k8s04pd7ps9cug85da2uaa695l5zqervd5</t>
+  </si>
+  <si>
+    <t>stars1tqz6k8s04pd7ps9cug85da2uaa695l5zp85qy5</t>
+  </si>
+  <si>
+    <t>juno1tqz6k8s04pd7ps9cug85da2uaa695l5zrfqxge</t>
+  </si>
+  <si>
+    <t>uptick18dfa2m6jwd53tdu5e03atqtw4ysfuwytm2q08u</t>
+  </si>
+  <si>
+    <t>omniflix1tqz6k8s04pd7ps9cug85da2uaa695l5zg9jycm</t>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jimmy668#7209</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -570,26 +596,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
@@ -641,6 +667,32 @@
         <v>26</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
@@ -649,17 +701,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -667,7 +719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -683,17 +735,17 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -701,7 +753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -717,17 +769,17 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -735,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -751,17 +803,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -769,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -785,17 +837,17 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -803,7 +855,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -811,12 +863,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -829,17 +881,17 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -847,7 +899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -855,12 +907,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -873,17 +925,17 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -891,7 +943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -899,12 +951,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -917,17 +969,17 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -935,7 +987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -943,12 +995,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -961,17 +1013,17 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -979,7 +1031,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -987,12 +1039,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1005,17 +1057,17 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1075,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1031,12 +1083,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1049,17 +1101,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1067,7 +1119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1083,17 +1135,17 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1109,12 +1161,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1127,17 +1179,17 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1145,7 +1197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -1153,12 +1205,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1171,24 +1223,24 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1205,26 +1257,26 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1241,26 +1293,26 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1277,26 +1329,26 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1313,18 +1365,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.90625" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1335,7 +1387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1354,18 +1406,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.90625" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1379,7 +1431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1401,18 +1453,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.90625" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1426,7 +1478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1448,18 +1500,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.90625" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1473,7 +1525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1495,20 +1547,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.90625" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1522,7 +1574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1544,17 +1596,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1562,7 +1614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -1578,17 +1630,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1596,7 +1648,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
2019jack stage2 add A7 to A20
</commit_message>
<xml_diff>
--- a/2019jack/evidence.xlsx
+++ b/2019jack/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cosmos\gon-evidence\2019jack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866E4DC6-5BBE-48FA-9E8D-AB411D484665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E285F37-11FE-49E7-BF8C-A3F45C77BA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="84">
   <si>
     <t>TeamName</t>
   </si>
@@ -82,21 +82,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
@@ -180,6 +165,203 @@
   </si>
   <si>
     <t>94E4BEE03CD46A473D46F24173C24183DFB11C8B5D31EAD21E2EF40712647148</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>punck01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>punck02</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>punck03</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>punck05</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>punck07</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>punck08</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9C1C5C3D7420B6DD8283560CC0C41F81ABC45F34132E2E1D5F8F1379570C5E65</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>81E722A3E554095FA01E9CC7863F26D901D10913AACE50D8142A39FB1BA92F35</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B298819DC4AAA452DD20FBC3DD387A8B9DFD330D81B2BD8952047D4076BCE125</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0E9F72E5FB90CF50998DAAD07DC5DF439C41F879C11A6B90713AC73D54CBB616</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>753CF6F58ECFA046A753C1FAC62E7944B23E40C06044C869850EE9EA3A55E59B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E876553AC86BCA95C8FD5599CD598E7A5433C9A3001F1CEFF7F74B677306A2AF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E8DC17F9069B5E00F045CE001F36549A3D23FA09F967A26170102C60BCCA0E97</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9140B9038F29ACD93605796560EA073464150D6DEE3A3BFB0317EF6F917E861A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9BE9F7DA4C067FCA09CC7CF15850212EB49F915F3286C6B7945719FE0EC3BB03</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A8BA5394F4DB41417987102CD8829F9F92B0CE18CFAC1B1ABAFFA620CC3E9A6B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8A70B43580E14D0DF5C7C8C58E38089C34EC046E6191B8024CDDD8AD43FF65FD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8FF2A1B09EF1583932C2C5D72CF1161FA7E8C3C016E1AFF45A48E7B51615C722</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1BA3AE481D7F5B8044085F41BD26704F153261217366DD489EB2A78FC848182E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8C5D534B6826E5EBE81A6341C13B65F8D12731832886CFAFDFBB7085CD40F425</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>131C505057B9239416F8B59B1C038DCD5321E3E6D134E559F2C0773F9E2BFF64</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>E06F96AD83FDC43D363B695DE2CDCB537A3F4892E11754F815AA3C83532F4429</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C3E1DADE4CB2A472FCF082FE20B04D790FD6543C7F5B4F5E3A63FAC8390AC75</t>
+  </si>
+  <si>
+    <t>8FFC75157FBB0377BCD5420DA4CBAF5063BC2302CFB13C729BFF6B531BB53310</t>
+  </si>
+  <si>
+    <t>14CB8D2B9FBA7EFDBF80F22FA5359073409B200A020FE846F3459645F53458F0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2BD8AF47B94314C890744DFD31226E438AB7ABDACEAF1DF8E322B6A6FF831A86</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>D0D666C7DC6D0EFE444ABF2D9813D0CE5299E88D9A457D340622B91E3A03BD80</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8792E56126B9D878F2F3B904836B147CDF5A2781BFEFA43CC0C7FB9B7B3E0633</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>46EC10850ECF63848BB0F50145AF30F253579327D6D10741DF9F32CC2732ABC6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9EA928F2221D5B42E5FD2155E8EF16358EA19B0805689F2DD8E1152F0E09F5CC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2E10F2F5CE98DC3E2C9BC93AF8E7C41DEE8009AD5DD87EAE7600D7134929648E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>98105C3E7D5E17BBDC49B875EB07F3325504FB4140C2E6AB7270D5733B7DDE4E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C48A9115B651322F14D6E61D4148F226255A9F8550F71FAF1D5871BF0CC4D5BC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>890A308B0385F02348EC1A254591E161DED8F39241D0630F46ACBAC7228A84F0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B466404C540193CF5DC894E14C700CB57BD6E502E287F42450EB23A8076C8F61</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10616F79F63B40A3D54AB44A18ABDD0E73FF9003D193BC53265FBEC845CA49F5</t>
+  </si>
+  <si>
+    <t>77D7F99A3274D5F13A3351384FA5C0768FD5C192464CD60CFB5419F8B7B19042</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>50E0E138DC1425A098CF29AE523DC72C93FF42601EB429591B4BC6E74D77E462</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>EF7099F621B21F89EF36C062890F123B71B4C4D37F55F96B144A81052E0DA5C5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2ADACC4AE45A2798535C409A11DFEB5796521A86169228440399116C3796769F</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>AB8BE3A8E6A3ACDA481620469C70AC25C4C1D796D92C8C412E91D32B7C65E711</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>F98EA0280F0A2E827C26917B4168A61C675EE609F1C828565244BC3A6C11B48E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/9EC59C445388057E70AEE5878B780200A607DF60FA94B8D65BE18D05FD798427</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/5BBB5AA4C7A6EBA260AE3ED1CB3DDA6E457DCBF36487851C95A7A8455B8A96A2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/4FED4D5920251145D8AE2856A0ED1CDDD5E2263387D8C9DB861D8B47278550CF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/BC28DC650D5914BA1E49C3C34FFC56A412F188632C4AA6EC3E6C473CB98B646A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/715DC4AE2A43B41BE5CC5C3489E5BB0A9C06D8CD377D723AA3785E24EA72F71F</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/B2987004376C9CAABDD918752F27A5DBE1A638B4068E990E8FD470B5F119B628</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -654,28 +836,28 @@
     </row>
     <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +871,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -706,10 +890,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +907,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -740,10 +926,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -757,7 +943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -774,10 +962,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -808,10 +998,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -823,9 +1013,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -842,20 +1034,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -867,9 +1073,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -886,20 +1094,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -911,9 +1133,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -930,20 +1154,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -955,9 +1193,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -974,20 +1214,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>55</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -999,9 +1253,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1018,20 +1274,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>59</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1043,9 +1313,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1062,20 +1334,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>63</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1108,10 +1394,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1123,9 +1409,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1142,20 +1430,50 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>67</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>68</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1167,9 +1485,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1186,20 +1506,50 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>73</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>74</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1224,12 +1574,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1260,12 +1610,12 @@
     </row>
     <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1296,12 +1646,12 @@
     </row>
     <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1332,12 +1682,12 @@
     </row>
     <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1378,24 +1728,24 @@
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1436,16 +1786,16 @@
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.5" x14ac:dyDescent="0.45">
@@ -1488,16 +1838,16 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1537,16 +1887,16 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1560,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1588,16 +1938,16 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1628,10 +1980,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1662,10 +2016,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 2019jack stage2 A19、A20 tx hash
</commit_message>
<xml_diff>
--- a/2019jack/evidence.xlsx
+++ b/2019jack/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cosmos\gon-evidence\2019jack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiexiaodong\Documents\2019jack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E285F37-11FE-49E7-BF8C-A3F45C77BA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E71159-6ABD-482E-9D41-1F0A84E7B0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="84">
   <si>
     <t>TeamName</t>
   </si>
@@ -314,54 +314,55 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>77D7F99A3274D5F13A3351384FA5C0768FD5C192464CD60CFB5419F8B7B19042</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>50E0E138DC1425A098CF29AE523DC72C93FF42601EB429591B4BC6E74D77E462</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>EF7099F621B21F89EF36C062890F123B71B4C4D37F55F96B144A81052E0DA5C5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2ADACC4AE45A2798535C409A11DFEB5796521A86169228440399116C3796769F</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>AB8BE3A8E6A3ACDA481620469C70AC25C4C1D796D92C8C412E91D32B7C65E711</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>F98EA0280F0A2E827C26917B4168A61C675EE609F1C828565244BC3A6C11B48E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/9EC59C445388057E70AEE5878B780200A607DF60FA94B8D65BE18D05FD798427</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/5BBB5AA4C7A6EBA260AE3ED1CB3DDA6E457DCBF36487851C95A7A8455B8A96A2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/4FED4D5920251145D8AE2856A0ED1CDDD5E2263387D8C9DB861D8B47278550CF</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/BC28DC650D5914BA1E49C3C34FFC56A412F188632C4AA6EC3E6C473CB98B646A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/715DC4AE2A43B41BE5CC5C3489E5BB0A9C06D8CD377D723AA3785E24EA72F71F</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/B2987004376C9CAABDD918752F27A5DBE1A638B4068E990E8FD470B5F119B628</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>10616F79F63B40A3D54AB44A18ABDD0E73FF9003D193BC53265FBEC845CA49F5</t>
-  </si>
-  <si>
-    <t>77D7F99A3274D5F13A3351384FA5C0768FD5C192464CD60CFB5419F8B7B19042</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>50E0E138DC1425A098CF29AE523DC72C93FF42601EB429591B4BC6E74D77E462</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>EF7099F621B21F89EF36C062890F123B71B4C4D37F55F96B144A81052E0DA5C5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2ADACC4AE45A2798535C409A11DFEB5796521A86169228440399116C3796769F</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>AB8BE3A8E6A3ACDA481620469C70AC25C4C1D796D92C8C412E91D32B7C65E711</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>F98EA0280F0A2E827C26917B4168A61C675EE609F1C828565244BC3A6C11B48E</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/9EC59C445388057E70AEE5878B780200A607DF60FA94B8D65BE18D05FD798427</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/5BBB5AA4C7A6EBA260AE3ED1CB3DDA6E457DCBF36487851C95A7A8455B8A96A2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/4FED4D5920251145D8AE2856A0ED1CDDD5E2263387D8C9DB861D8B47278550CF</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/BC28DC650D5914BA1E49C3C34FFC56A412F188632C4AA6EC3E6C473CB98B646A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/715DC4AE2A43B41BE5CC5C3489E5BB0A9C06D8CD377D723AA3785E24EA72F71F</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/B2987004376C9CAABDD918752F27A5DBE1A638B4068E990E8FD470B5F119B628</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -872,7 +873,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -890,7 +891,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
@@ -908,7 +909,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -926,7 +927,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>37</v>
@@ -944,7 +945,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -962,7 +963,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>38</v>
@@ -980,7 +981,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -998,7 +999,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>39</v>
@@ -1016,7 +1017,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1077,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1136,7 +1137,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1197,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1257,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1316,7 +1317,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1413,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1468,9 +1469,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>71</v>
+    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>42</v>
@@ -1485,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1507,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>32</v>
@@ -1514,7 +1515,7 @@
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>44</v>
@@ -1522,23 +1523,23 @@
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>42</v>
@@ -1546,10 +1547,26 @@
     </row>
     <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1962,7 +1979,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1980,7 +1997,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>34</v>
@@ -1998,7 +2015,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2016,7 +2033,7 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
update 2019jack A1-A6 task
</commit_message>
<xml_diff>
--- a/2019jack/evidence.xlsx
+++ b/2019jack/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiexiaodong\Documents\2019jack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E71159-6ABD-482E-9D41-1F0A84E7B0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F624BBA3-39D5-4B3E-B5D3-F3F62A073354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="95">
   <si>
     <t>TeamName</t>
   </si>
@@ -120,54 +120,18 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>6CA7C7C691D81DF2A31B38D073C7F0146C1DFDFB4A169A856A28A3B1D3DE3912</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>BA82EC90C33D12E0BD3DFA55042E401EAEEABAEA017EA0919E3ACDD92762B27D</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>brain01</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>B65AFDC9AC373A75ACF0C5987962BEFD347C6FC912BFC0BEFCBB6F6E0F607932</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>brain02</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>5889B4256C555733526F6D30062B036A35F53CAE984955FCA232AE527D3EE905</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>uni-6</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>088839C8744903BEE192AC6A1D0E5FF777F4D15866F17C0722C1141F1F5BCD44</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>gon-flixnet-1</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>449DC0339CF82424B39714F798DDB3D46DB9ACBF211FE97E88E5BA09A37D6EF5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>gon-irishub-1</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>94E4BEE03CD46A473D46F24173C24183DFB11C8B5D31EAD21E2EF40712647148</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>punck01</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -363,6 +327,84 @@
   </si>
   <si>
     <t>10616F79F63B40A3D54AB44A18ABDD0E73FF9003D193BC53265FBEC845CA49F5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A2D4C68A15AAC3BBBF676D272B0D6EEBB6E60D9C77838F531F9A9AEBBF359A59</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>dongjohn2023</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>41647A23805548B8584ED2E1A80368F145DF202097B8939BC12E215E9E92A48C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>jack1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>096CD4D076AF4A17D423C5AC414C155E6E2E74A50598580165C6546DB0A5268A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>jack2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>67764BD6B9F880064BF58892DE1C96D5D0E1A428521565C284402EC3D262D372</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>jack3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3AEE2DA8DB0ECF438DDCF5590608ECFB98D4F173938C75DC716DA9E115A33CF2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>jack4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>8B0CCF54973E14EE9B319D5E931B459CE3CF02083583C8DD1488DE292E385285</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>jack5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C20A806B6C8B0C70E722BEDADB699FE56DD13C49B2EF951721CAFBEC2912FB17</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stars145jcuw9zz5s5mfmqj860e6flcf07w4dmxxvcuxdnecj2vjj9qmks2p3uja</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>98F5AEF1719D5A128ABD8E0130E8EF46AE68192118EC244CFDFAE1F9EAE128E3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/3AD0E6222502938FC60FE999B7D7B587EB879601B1273C0EA10463A303057372</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>41D295E80969B8FE7A74AE10D907873C08648694F82E28F9D5F6DCE60A8836CD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>928DC31776EF03F5D9675CF0D8DB702687754E2EA0CB84135D5A79A0053BBA23</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -370,7 +412,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -407,6 +449,17 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -440,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -448,6 +501,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -891,10 +950,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -927,10 +986,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -963,10 +1022,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -999,10 +1058,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1035,34 +1094,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1095,34 +1154,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1155,34 +1214,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1215,34 +1274,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1275,34 +1334,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1335,34 +1394,34 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1436,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1395,10 +1454,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1431,50 +1490,50 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1488,7 +1547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1507,66 +1566,66 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1720,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1745,24 +1804,57 @@
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1777,7 +1869,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1803,16 +1895,16 @@
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.5" x14ac:dyDescent="0.45">
@@ -1830,7 +1922,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1855,16 +1947,16 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +1971,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1902,18 +1994,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>80</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1927,8 +2019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1936,7 +2028,7 @@
     <col min="1" max="1" width="17.90625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.3">
@@ -1955,16 +2047,16 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>78</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1997,10 +2089,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2033,10 +2125,10 @@
     </row>
     <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2019jack update B1-B2 task
</commit_message>
<xml_diff>
--- a/2019jack/evidence.xlsx
+++ b/2019jack/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiexiaodong\Documents\2019jack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F624BBA3-39D5-4B3E-B5D3-F3F62A073354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DA48E9-273F-441E-84D6-31D2FE6ACA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="12" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="90">
   <si>
     <t>TeamName</t>
   </si>
@@ -330,81 +330,63 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>A2D4C68A15AAC3BBBF676D272B0D6EEBB6E60D9C77838F531F9A9AEBBF359A59</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>dongjohn2023</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>41647A23805548B8584ED2E1A80368F145DF202097B8939BC12E215E9E92A48C</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>jack1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>096CD4D076AF4A17D423C5AC414C155E6E2E74A50598580165C6546DB0A5268A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>jack2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>67764BD6B9F880064BF58892DE1C96D5D0E1A428521565C284402EC3D262D372</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>jack3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>3AEE2DA8DB0ECF438DDCF5590608ECFB98D4F173938C75DC716DA9E115A33CF2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>jack4</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>8B0CCF54973E14EE9B319D5E931B459CE3CF02083583C8DD1488DE292E385285</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>jack5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>C20A806B6C8B0C70E722BEDADB699FE56DD13C49B2EF951721CAFBEC2912FB17</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stars145jcuw9zz5s5mfmqj860e6flcf07w4dmxxvcuxdnecj2vjj9qmks2p3uja</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>elgafar-1</t>
-  </si>
-  <si>
-    <t>98F5AEF1719D5A128ABD8E0130E8EF46AE68192118EC244CFDFAE1F9EAE128E3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/3AD0E6222502938FC60FE999B7D7B587EB879601B1273C0EA10463A303057372</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>uptick_7000-2</t>
-  </si>
-  <si>
-    <t>41D295E80969B8FE7A74AE10D907873C08648694F82E28F9D5F6DCE60A8836CD</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>928DC31776EF03F5D9675CF0D8DB702687754E2EA0CB84135D5A79A0053BBA23</t>
+    <t>6CA7C7C691D81DF2A31B38D073C7F0146C1DFDFB4A169A856A28A3B1D3DE3912</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BA82EC90C33D12E0BD3DFA55042E401EAEEABAEA017EA0919E3ACDD92762B27D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>brain01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B65AFDC9AC373A75ACF0C5987962BEFD347C6FC912BFC0BEFCBB6F6E0F607932</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>brain02</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>5889B4256C555733526F6D30062B036A35F53CAE984955FCA232AE527D3EE905</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>juno1mmfe293cwm3jr7uqufs0ll3lj622vg6klpnyjv0rupyqk0m89t9s6nvxrw</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>088839C8744903BEE192AC6A1D0E5FF777F4D15866F17C0722C1141F1F5BCD44</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/BF27F1A5A3EE62764772D56E3B213FACAA6AC1DF241813A6F6B1A5CDD49E9480</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>449DC0339CF82424B39714F798DDB3D46DB9ACBF211FE97E88E5BA09A37D6EF5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>94E4BEE03CD46A473D46F24173C24183DFB11C8B5D31EAD21E2EF40712647148</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B343C0E3B3F1855E6AC459E68702E0A32826E1E61EDF783049F4121373C98DAA</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAD5F5F83D21CD900CC7EFB17A3CE6B6E0D0E572E95201CB8714A8C68DAF3A54</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B6D173C66352078ECEE360E4F4C6988A21474D8C6C1C6DE16612DF4D61D125B5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>77F3963DB2F285BF563A0C346B17C289463EC2C0A9ACB9922399D67D5FD7AA05</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -968,7 +950,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1418,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1439,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1530,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1639,7 +1621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1649,13 +1633,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1673,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1685,13 +1669,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1782,7 +1766,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1804,58 +1788,40 @@
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>82</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1869,7 +1835,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1895,16 +1861,16 @@
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.5" x14ac:dyDescent="0.45">
@@ -1922,7 +1888,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1947,16 +1913,16 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1971,7 +1937,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1996,16 +1962,16 @@
     </row>
     <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2019,8 +1985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2047,16 +2013,16 @@
     </row>
     <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2071,7 +2037,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2019jack update B5-B8 task
</commit_message>
<xml_diff>
--- a/2019jack/evidence.xlsx
+++ b/2019jack/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiexiaodong\Documents\2019jack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DA48E9-273F-441E-84D6-31D2FE6ACA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50091CDB-B7AF-469C-90D8-801B84FCB98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="12" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="14" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,15 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
+    <sheet name="B8" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="96">
   <si>
     <t>TeamName</t>
   </si>
@@ -387,6 +389,30 @@
   </si>
   <si>
     <t>77F3963DB2F285BF563A0C346B17C289463EC2C0A9ACB9922399D67D5FD7AA05</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DA89BF3CB114E5958AD762BACD4C4C6A343FEAC2C0EDAB23737610D6A9768DD0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>7FA45E82327B42710FF4423E4CC80DE7F60EFF7EB1E9C4967809A64631A47467</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>72620E9A66C080EE14B536E210AC3F6B71C3D5A401AFA6C595A0A4590160D065</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>34E75DD07859B6FF24E41E380727E9668E6BA46126FA85AD58AE62219DE2AB57</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C449B60765751390553D11172C966921A93CBA3A59A27B085BBA9C7DCB0A9FD3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>500F1C46E512219F1B9D8CF812AEE703795F41FB8144496E72C257ADA5B7B7C4</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1657,7 +1683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1694,7 +1720,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1705,13 +1731,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1730,7 +1756,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1741,13 +1767,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1758,6 +1784,68 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A50857-8945-4655-9FBB-E1791C611FA5}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB72AFF8-9B7A-4867-AC67-B4F9D33A5326}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>